<commit_message>
modify headers to avoid using _
</commit_message>
<xml_diff>
--- a/jets/expdata/10003.xlsx
+++ b/jets/expdata/10003.xlsx
@@ -1,39 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yiyu/Google Drive/ing/jefferson lab/scholarship/monte carlo/fitpack2/database/jet/expdata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4CA96E-A885-D240-AF9B-BBA0185A3685}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="17020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+  <si>
+    <t>idx</t>
+  </si>
   <si>
     <t>col</t>
+  </si>
+  <si>
+    <t>particles-in</t>
   </si>
   <si>
     <t>RS</t>
   </si>
   <si>
+    <t>pt-min</t>
+  </si>
+  <si>
+    <t>pt-max</t>
+  </si>
+  <si>
     <t>pT</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>eta-min</t>
+  </si>
+  <si>
+    <t>eta-max</t>
+  </si>
+  <si>
+    <t>cone-radius</t>
   </si>
   <si>
     <t>obs</t>
@@ -45,80 +58,397 @@
     <t>value</t>
   </si>
   <si>
-    <t>pt_min</t>
-  </si>
-  <si>
-    <t>pt_max</t>
-  </si>
-  <si>
-    <t>tau</t>
-  </si>
-  <si>
-    <t>plot_factor</t>
-  </si>
-  <si>
     <t>stat_u</t>
   </si>
   <si>
     <t>sys_c</t>
   </si>
   <si>
-    <t>idx</t>
+    <t>plot-factor</t>
+  </si>
+  <si>
+    <t>star</t>
   </si>
   <si>
     <t>pp</t>
   </si>
   <si>
-    <t>pb</t>
-  </si>
-  <si>
-    <t>star</t>
-  </si>
-  <si>
-    <t>eta_min</t>
-  </si>
-  <si>
-    <t>eta_max</t>
-  </si>
-  <si>
-    <t>cone_radius</t>
-  </si>
-  <si>
     <t>&lt;d2_sigma_over_2_pi_d_y_d_pt&gt;</t>
   </si>
   <si>
-    <t>particles_in</t>
+    <t>pb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="17"/>
       <color rgb="FF000000"/>
       <name val="Gabriola"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="26"/>
       <color rgb="FF000000"/>
       <name val="Gabriola"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -126,33 +456,319 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -201,7 +817,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -234,26 +850,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -286,23 +885,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,102 +1026,96 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:Q123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2:N6"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.71120689655172" defaultRowHeight="24.4"/>
   <cols>
-    <col min="1" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="12" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="1016" width="10.28515625" customWidth="1"/>
+    <col min="1" max="2" width="10.2844827586207" customWidth="1"/>
+    <col min="3" max="3" width="13.8534482758621" customWidth="1"/>
+    <col min="4" max="8" width="10.2844827586207" customWidth="1"/>
+    <col min="9" max="9" width="14.8534482758621" customWidth="1"/>
+    <col min="10" max="11" width="15.5689655172414" customWidth="1"/>
+    <col min="12" max="12" width="35.7112068965517" customWidth="1"/>
+    <col min="13" max="13" width="10.2844827586207" customWidth="1"/>
+    <col min="14" max="16" width="17" customWidth="1"/>
+    <col min="17" max="17" width="13.1422413793103" customWidth="1"/>
+    <col min="18" max="1016" width="10.2844827586207" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" ht="35.6" spans="1:17">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" ht="35.6" spans="1:17">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1">
         <v>200</v>
@@ -555,7 +1131,7 @@
       </c>
       <c r="H2" s="1">
         <f>2*G2/D2</f>
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="I2" s="1">
         <v>0.2</v>
@@ -570,30 +1146,30 @@
         <v>19</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="3">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2">
         <v>9300000</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="3">
         <v>300000</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="3">
         <v>4500000</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" ht="35.6" spans="1:17">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
         <v>200</v>
@@ -609,7 +1185,7 @@
       </c>
       <c r="H3" s="1">
         <f>2*G3/D3</f>
-        <v>6.8000000000000005E-2</v>
+        <v>0.068</v>
       </c>
       <c r="I3" s="1">
         <v>0.2</v>
@@ -624,30 +1200,30 @@
         <v>19</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="3">
+        <v>20</v>
+      </c>
+      <c r="N3" s="2">
         <v>2700000</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="3">
         <v>100000</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="3">
         <v>1300000</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" ht="35.6" spans="1:17">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>200</v>
@@ -656,14 +1232,14 @@
         <v>7.6</v>
       </c>
       <c r="F4" s="1">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="G4" s="1">
-        <v>8.3000000000000007</v>
+        <v>8.3</v>
       </c>
       <c r="H4" s="1">
         <f>2*G4/D4</f>
-        <v>8.3000000000000004E-2</v>
+        <v>0.083</v>
       </c>
       <c r="I4" s="1">
         <v>0.2</v>
@@ -678,36 +1254,36 @@
         <v>19</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="3">
+        <v>20</v>
+      </c>
+      <c r="N4" s="2">
         <v>670000</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="3">
         <v>50000</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="3">
         <v>320000</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" ht="35.6" spans="1:17">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1">
         <v>200</v>
       </c>
       <c r="E5" s="1">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="F5" s="1">
         <v>11.4</v>
@@ -717,7 +1293,7 @@
       </c>
       <c r="H5" s="1">
         <f>2*G5/D5</f>
-        <v>0.10300000000000001</v>
+        <v>0.103</v>
       </c>
       <c r="I5" s="1">
         <v>0.2</v>
@@ -732,30 +1308,30 @@
         <v>19</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N5" s="3">
+        <v>20</v>
+      </c>
+      <c r="N5" s="2">
         <v>184000</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="3">
         <v>24000</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="3">
         <v>88000</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" ht="35.6" spans="1:17">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1">
         <v>200</v>
@@ -786,22 +1362,22 @@
         <v>19</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N6" s="3">
+        <v>20</v>
+      </c>
+      <c r="N6" s="2">
         <v>51000</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="3">
         <v>11000</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="3">
         <v>24000</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" ht="35.6" spans="1:17">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -818,9 +1394,9 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" ht="35.6" spans="1:17">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -837,9 +1413,9 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" ht="35.6" spans="1:17">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -856,9 +1432,9 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" ht="35.6" spans="1:17">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -875,9 +1451,9 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" ht="35.6" spans="1:17">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -894,9 +1470,9 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="2"/>
-    </row>
-    <row r="21" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" ht="35.6" spans="1:17">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -913,9 +1489,9 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" ht="35.6" spans="1:17">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -932,9 +1508,9 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" ht="35.6" spans="1:17">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -951,9 +1527,9 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" ht="35.6" spans="1:17">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -970,9 +1546,9 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" ht="35.6" spans="1:17">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -989,9 +1565,9 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" ht="35.6" spans="1:17">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1008,9 +1584,9 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" ht="35.6" spans="1:17">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1027,9 +1603,9 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" ht="35.6" spans="1:17">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1046,9 +1622,9 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="2"/>
-    </row>
-    <row r="29" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" ht="35.6" spans="1:17">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1065,9 +1641,9 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="2"/>
-    </row>
-    <row r="30" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="30" ht="35.6" spans="1:17">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1084,9 +1660,9 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-      <c r="Q30" s="2"/>
-    </row>
-    <row r="31" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q30" s="3"/>
+    </row>
+    <row r="31" ht="35.6" spans="1:17">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1103,9 +1679,9 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="Q31" s="2"/>
-    </row>
-    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" ht="35.6" spans="1:17">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1122,9 +1698,9 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
-      <c r="Q32" s="2"/>
-    </row>
-    <row r="33" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q32" s="3"/>
+    </row>
+    <row r="33" ht="35.6" spans="1:17">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1141,9 +1717,9 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
-      <c r="Q33" s="2"/>
-    </row>
-    <row r="34" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q33" s="3"/>
+    </row>
+    <row r="34" ht="35.6" spans="1:17">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1162,7 +1738,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" ht="35.6" spans="1:17">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1181,7 +1757,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" ht="35.6" spans="1:17">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1200,7 +1776,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" ht="35.6" spans="1:17">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1219,7 +1795,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" ht="35.6" spans="1:17">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1238,7 +1814,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" ht="35.6" spans="1:17">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1257,7 +1833,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" ht="35.6" spans="1:17">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1276,7 +1852,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" ht="35.6" spans="1:17">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1295,7 +1871,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" ht="35.6" spans="1:17">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1314,7 +1890,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" ht="35.6" spans="1:17">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1333,7 +1909,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" ht="35.6" spans="1:17">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1352,7 +1928,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" ht="35.6" spans="1:17">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1371,7 +1947,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" ht="35.6" spans="1:17">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1390,7 +1966,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" ht="35.6" spans="1:17">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1409,7 +1985,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" ht="35.6" spans="1:17">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1428,7 +2004,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" ht="35.6" spans="1:17">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1447,7 +2023,7 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" ht="35.6" spans="1:17">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1466,7 +2042,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" ht="35.6" spans="1:17">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1485,7 +2061,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" ht="35.6" spans="1:17">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1504,7 +2080,7 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" ht="35.6" spans="1:17">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1523,7 +2099,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" ht="35.6" spans="1:17">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1542,7 +2118,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" ht="35.6" spans="1:17">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1561,7 +2137,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
     </row>
-    <row r="56" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" ht="35.6" spans="1:17">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1580,7 +2156,7 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
     </row>
-    <row r="57" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" ht="35.6" spans="1:17">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1599,7 +2175,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
     </row>
-    <row r="58" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" ht="35.6" spans="1:17">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1618,7 +2194,7 @@
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
     </row>
-    <row r="59" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" ht="35.6" spans="1:17">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1637,7 +2213,7 @@
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
     </row>
-    <row r="60" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" ht="35.6" spans="1:17">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1656,7 +2232,7 @@
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
     </row>
-    <row r="61" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" ht="35.6" spans="1:17">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1675,7 +2251,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" ht="35.6" spans="1:17">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1694,7 +2270,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" ht="35.6" spans="1:17">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1713,7 +2289,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" ht="35.6" spans="1:17">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1732,7 +2308,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" ht="35.6" spans="1:17">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1751,7 +2327,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" ht="35.6" spans="1:17">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1770,7 +2346,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" ht="35.6" spans="1:17">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1789,7 +2365,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" ht="35.6" spans="1:17">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1808,7 +2384,7 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" ht="35.6" spans="1:17">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1827,7 +2403,7 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" ht="35.6" spans="1:17">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1846,7 +2422,7 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" ht="35.6" spans="1:17">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1865,7 +2441,7 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" ht="35.6" spans="1:17">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1884,7 +2460,7 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" ht="35.6" spans="1:17">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1903,7 +2479,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" ht="35.6" spans="1:17">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1922,7 +2498,7 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
     </row>
-    <row r="75" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" ht="35.6" spans="1:17">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1941,7 +2517,7 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
     </row>
-    <row r="76" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" ht="35.6" spans="1:17">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1960,7 +2536,7 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
     </row>
-    <row r="77" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" ht="35.6" spans="1:17">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1979,7 +2555,7 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
     </row>
-    <row r="78" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" ht="35.6" spans="1:17">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1998,7 +2574,7 @@
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
     </row>
-    <row r="79" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" ht="35.6" spans="1:17">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2017,7 +2593,7 @@
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
     </row>
-    <row r="80" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" ht="35.6" spans="1:17">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2036,7 +2612,7 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
     </row>
-    <row r="81" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" ht="35.6" spans="1:17">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2055,7 +2631,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" ht="35.6" spans="1:17">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2074,7 +2650,7 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
     </row>
-    <row r="83" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" ht="35.6" spans="1:17">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2093,7 +2669,7 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" ht="35.6" spans="1:17">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2112,7 +2688,7 @@
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
     </row>
-    <row r="85" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" ht="35.6" spans="1:17">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2131,7 +2707,7 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
     </row>
-    <row r="86" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" ht="35.6" spans="1:17">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2150,7 +2726,7 @@
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
     </row>
-    <row r="87" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" ht="35.6" spans="1:17">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2169,7 +2745,7 @@
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
     </row>
-    <row r="88" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" ht="35.6" spans="1:17">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2188,7 +2764,7 @@
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
     </row>
-    <row r="89" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" ht="35.6" spans="1:17">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2207,7 +2783,7 @@
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
     </row>
-    <row r="90" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" ht="35.6" spans="1:17">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2226,7 +2802,7 @@
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
     </row>
-    <row r="91" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" ht="35.6" spans="1:17">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2245,7 +2821,7 @@
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
     </row>
-    <row r="92" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" ht="35.6" spans="1:17">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2264,7 +2840,7 @@
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
     </row>
-    <row r="93" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" ht="35.6" spans="1:17">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2283,7 +2859,7 @@
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
     </row>
-    <row r="94" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" ht="35.6" spans="1:17">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2302,7 +2878,7 @@
       <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
     </row>
-    <row r="95" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" ht="35.6" spans="1:17">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2321,7 +2897,7 @@
       <c r="P95" s="1"/>
       <c r="Q95" s="1"/>
     </row>
-    <row r="96" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" ht="35.6" spans="1:17">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2340,7 +2916,7 @@
       <c r="P96" s="1"/>
       <c r="Q96" s="1"/>
     </row>
-    <row r="97" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" ht="35.6" spans="1:17">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2359,7 +2935,7 @@
       <c r="P97" s="1"/>
       <c r="Q97" s="1"/>
     </row>
-    <row r="98" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" ht="35.6" spans="1:17">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2378,7 +2954,7 @@
       <c r="P98" s="1"/>
       <c r="Q98" s="1"/>
     </row>
-    <row r="99" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" ht="35.6" spans="1:17">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2397,7 +2973,7 @@
       <c r="P99" s="1"/>
       <c r="Q99" s="1"/>
     </row>
-    <row r="100" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" ht="35.6" spans="1:17">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2416,7 +2992,7 @@
       <c r="P100" s="1"/>
       <c r="Q100" s="1"/>
     </row>
-    <row r="101" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" ht="35.6" spans="1:17">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2435,7 +3011,7 @@
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
     </row>
-    <row r="102" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" ht="35.6" spans="1:17">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2454,7 +3030,7 @@
       <c r="P102" s="1"/>
       <c r="Q102" s="1"/>
     </row>
-    <row r="103" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" ht="35.6" spans="1:17">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2473,7 +3049,7 @@
       <c r="P103" s="1"/>
       <c r="Q103" s="1"/>
     </row>
-    <row r="104" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" ht="35.6" spans="1:17">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2492,7 +3068,7 @@
       <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
     </row>
-    <row r="105" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" ht="35.6" spans="1:17">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2511,7 +3087,7 @@
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
     </row>
-    <row r="106" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" ht="35.6" spans="1:17">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2530,7 +3106,7 @@
       <c r="P106" s="1"/>
       <c r="Q106" s="1"/>
     </row>
-    <row r="107" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" ht="35.6" spans="1:17">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2549,7 +3125,7 @@
       <c r="P107" s="1"/>
       <c r="Q107" s="1"/>
     </row>
-    <row r="108" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" ht="35.6" spans="1:17">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2568,7 +3144,7 @@
       <c r="P108" s="1"/>
       <c r="Q108" s="1"/>
     </row>
-    <row r="109" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" ht="35.6" spans="1:17">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2587,7 +3163,7 @@
       <c r="P109" s="1"/>
       <c r="Q109" s="1"/>
     </row>
-    <row r="110" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" ht="35.6" spans="1:17">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2606,7 +3182,7 @@
       <c r="P110" s="1"/>
       <c r="Q110" s="1"/>
     </row>
-    <row r="111" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" ht="35.6" spans="1:17">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2625,7 +3201,7 @@
       <c r="P111" s="1"/>
       <c r="Q111" s="1"/>
     </row>
-    <row r="112" spans="1:17" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" ht="35.6" spans="1:16">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2640,7 +3216,7 @@
       <c r="O112" s="1"/>
       <c r="P112" s="1"/>
     </row>
-    <row r="113" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" ht="35.6" spans="1:16">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2655,7 +3231,7 @@
       <c r="O113" s="1"/>
       <c r="P113" s="1"/>
     </row>
-    <row r="114" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" ht="35.6" spans="1:16">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2670,7 +3246,7 @@
       <c r="O114" s="1"/>
       <c r="P114" s="1"/>
     </row>
-    <row r="115" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" ht="35.6" spans="1:16">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2685,7 +3261,7 @@
       <c r="O115" s="1"/>
       <c r="P115" s="1"/>
     </row>
-    <row r="116" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" ht="35.6" spans="1:16">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2700,7 +3276,7 @@
       <c r="O116" s="1"/>
       <c r="P116" s="1"/>
     </row>
-    <row r="117" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" ht="35.6" spans="1:16">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2715,7 +3291,7 @@
       <c r="O117" s="1"/>
       <c r="P117" s="1"/>
     </row>
-    <row r="118" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" ht="35.6" spans="1:16">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2730,7 +3306,7 @@
       <c r="O118" s="1"/>
       <c r="P118" s="1"/>
     </row>
-    <row r="119" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" ht="35.6" spans="1:16">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2745,7 +3321,7 @@
       <c r="O119" s="1"/>
       <c r="P119" s="1"/>
     </row>
-    <row r="120" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" ht="35.6" spans="1:16">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2760,7 +3336,7 @@
       <c r="O120" s="1"/>
       <c r="P120" s="1"/>
     </row>
-    <row r="121" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" ht="35.6" spans="1:16">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2775,7 +3351,7 @@
       <c r="O121" s="1"/>
       <c r="P121" s="1"/>
     </row>
-    <row r="122" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" ht="35.6" spans="1:16">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2790,7 +3366,7 @@
       <c r="O122" s="1"/>
       <c r="P122" s="1"/>
     </row>
-    <row r="123" spans="1:16" ht="51" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" ht="35.6" spans="1:16">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2806,7 +3382,8 @@
       <c r="P123" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>